<commit_message>
Fix the term IRI for Stereo-seq
</commit_message>
<xml_diff>
--- a/stereo-seq/latest/stereo-seq.xlsx
+++ b/stereo-seq/latest/stereo-seq.xlsx
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="339">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -210,7 +210,7 @@
     <t>Stereo-seq</t>
   </si>
   <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000434</t>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
   </si>
   <si>
     <t>Visium (with probes)</t>
@@ -303,6 +303,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
   </si>
   <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -1149,7 +1155,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-06-02T07:32:43-07:00</t>
+    <t>2025-06-10T10:07:06-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1275,37 +1281,37 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2">
@@ -1313,13 +1319,13 @@
         <v>20</v>
       </c>
       <c r="O2" t="s" s="16">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="9">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$41</formula1>
+      <formula1>'dataset_type'!$A$1:$A$42</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1356,7 +1362,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1688,6 +1694,14 @@
       </c>
       <c r="B41" t="s" s="0">
         <v>85</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1705,130 +1719,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1846,12 +1860,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1869,218 +1883,218 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2098,546 +2112,546 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -2655,42 +2669,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2708,26 +2722,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -2751,16 +2765,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2">
@@ -2768,13 +2782,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>